<commit_message>
add implementation of all measures.
</commit_message>
<xml_diff>
--- a/data/system/entity_template.xlsx
+++ b/data/system/entity_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aznarsig/Documents/Python/climada_python/data/system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{541B7F0A-6765-014C-9A4C-62BF4C6DD8CF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C49CBED-F038-3942-8736-FC3AA5899C17}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="766" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="_discounting_sheet" sheetId="6" r:id="rId6"/>
     <sheet name="names" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -696,7 +696,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -741,12 +741,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>events with frequencies higher than cutoff are ignored. If set to zero, all events are used (default=0).
-This parameter can be used to reflect effects of prevention measures like e.g. a 50yr flood defense (in which case one sets this parameter to 1/50)</t>
+          <t xml:space="preserve">events with frequencies higher than cutoff are ignored. If set to zero, all events are used (default=0).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>This parameter can be used to reflect effects of prevention measures like e.g. a 50yr flood defense (in which case one sets this parameter to 1/50)</t>
         </r>
       </text>
     </comment>
@@ -755,11 +774,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">In order to use a measure-specific hazard event set, the user can specifiy the filename (enter nil not to use this option). If a filename is specified, it is searched for in the same folder as the hazard used for the rest of the analysis. If a filename with path is specified, the measure-specific hazard can reside any place. Please note that if the same measures file is used with hazard sets representative for different times, e.g. once a hazard set representative for today, then one for 2030, the measure-specific hazard event set is likely not to be the same. But usually, the entity file is for a specific time (e.g. 2030), and so will be the measure-specific hazard event set specified within.
+          <t xml:space="preserve">In order to use a measure-specific hazard event set, the user can specifiy the filename (enter nil not to use this option). Provide the filename with absolute path and h5 format (file should have been generated by CLIMADA write_hdf5()). Please note that if the same measures file is used with hazard sets representative for different times, e.g. once a hazard set representative for today, then one for 2030, the measure-specific hazard event set is likely not to be the same. But usually, the entity file is for a specific time (e.g. 2030), and so will be the measure-specific hazard event set specified within.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -769,13 +798,41 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>MDD=orig_MDD*a+b
-The original Mean Damage Degree(the damage for a given intensity at an affected asset) is linearly transformed
-default=1</t>
+          <t xml:space="preserve">MDD=orig_MDD*a+b
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The original Mean Damage Degree(the damage for a given intensity at an affected asset) is linearly transformed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>default=1</t>
         </r>
       </text>
     </comment>
@@ -784,13 +841,41 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>MDD=orig_MDD*a+b
-The original Mean Damage Degree(the damage for a given intensity at an affected asset) is linearly transformed
-default=0</t>
+          <t xml:space="preserve">MDD=orig_MDD*a+b
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">The original Mean Damage Degree(the damage for a given intensity at an affected asset) is linearly transformed
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>default=0</t>
         </r>
       </text>
     </comment>
@@ -848,12 +933,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t>OPTIONAL
-Use a measure specific asset file</t>
+          <t xml:space="preserve">OPTIONAL
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Use a measure specific asset file in h5 format (generated by CLIMADA)</t>
         </r>
       </text>
     </comment>
@@ -1863,7 +1967,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1"/>
@@ -1882,6 +1985,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="169" fontId="1" fillId="4" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -3204,10 +3308,10 @@
       <c r="E1" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="75" t="s">
+      <c r="F1" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="75" t="s">
+      <c r="G1" s="74" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3227,10 +3331,10 @@
       <c r="E2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="76" t="s">
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3250,10 +3354,10 @@
       <c r="E3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="76" t="s">
+      <c r="G3" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3273,10 +3377,10 @@
       <c r="E4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="76" t="s">
+      <c r="G4" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3296,10 +3400,10 @@
       <c r="E5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="76" t="s">
+      <c r="G5" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3319,10 +3423,10 @@
       <c r="E6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="76" t="s">
+      <c r="G6" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3342,10 +3446,10 @@
       <c r="E7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="76" t="s">
+      <c r="G7" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3365,10 +3469,10 @@
       <c r="E8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="76" t="s">
+      <c r="F8" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="76" t="s">
+      <c r="G8" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3388,10 +3492,10 @@
       <c r="E9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="76" t="s">
+      <c r="F9" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="76" t="s">
+      <c r="G9" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3411,10 +3515,10 @@
       <c r="E10" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="76" t="s">
+      <c r="G10" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3434,10 +3538,10 @@
       <c r="E11" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="76" t="s">
+      <c r="F11" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="76" t="s">
+      <c r="G11" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3457,10 +3561,10 @@
       <c r="E12" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="76" t="s">
+      <c r="F12" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="76" t="s">
+      <c r="G12" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3480,10 +3584,10 @@
       <c r="E13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="76" t="s">
+      <c r="F13" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3503,10 +3607,10 @@
       <c r="E14" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="76" t="s">
+      <c r="F14" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="76" t="s">
+      <c r="G14" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3526,10 +3630,10 @@
       <c r="E15" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="76" t="s">
+      <c r="F15" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="76" t="s">
+      <c r="G15" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3549,10 +3653,10 @@
       <c r="E16" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="76" t="s">
+      <c r="F16" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="76" t="s">
+      <c r="G16" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3572,10 +3676,10 @@
       <c r="E17" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="76" t="s">
+      <c r="F17" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="76" t="s">
+      <c r="G17" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3595,10 +3699,10 @@
       <c r="E18" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="76" t="s">
+      <c r="F18" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="76" t="s">
+      <c r="G18" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3618,10 +3722,10 @@
       <c r="E19" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="76" t="s">
+      <c r="F19" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="76" t="s">
+      <c r="G19" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3641,10 +3745,10 @@
       <c r="E20" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="76" t="s">
+      <c r="F20" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G20" s="76" t="s">
+      <c r="G20" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3664,10 +3768,10 @@
       <c r="E21" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="76" t="s">
+      <c r="F21" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="76" t="s">
+      <c r="G21" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3687,10 +3791,10 @@
       <c r="E22" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="76" t="s">
+      <c r="F22" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G22" s="76" t="s">
+      <c r="G22" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3710,10 +3814,10 @@
       <c r="E23" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="76" t="s">
+      <c r="F23" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="76" t="s">
+      <c r="G23" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3733,10 +3837,10 @@
       <c r="E24" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="76" t="s">
+      <c r="F24" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="76" t="s">
+      <c r="G24" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3756,10 +3860,10 @@
       <c r="E25" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="76" t="s">
+      <c r="F25" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="76" t="s">
+      <c r="G25" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3779,10 +3883,10 @@
       <c r="E26" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="76" t="s">
+      <c r="F26" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G26" s="76" t="s">
+      <c r="G26" s="75" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3802,10 +3906,10 @@
       <c r="E27" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="76" t="s">
+      <c r="F27" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="76" t="s">
+      <c r="G27" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3825,10 +3929,10 @@
       <c r="E28" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="76" t="s">
+      <c r="F28" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="76" t="s">
+      <c r="G28" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3848,10 +3952,10 @@
       <c r="E29" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="76" t="s">
+      <c r="F29" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="76" t="s">
+      <c r="G29" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3871,10 +3975,10 @@
       <c r="E30" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F30" s="76" t="s">
+      <c r="F30" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="76" t="s">
+      <c r="G30" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3894,10 +3998,10 @@
       <c r="E31" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="76" t="s">
+      <c r="F31" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="76" t="s">
+      <c r="G31" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3917,10 +4021,10 @@
       <c r="E32" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F32" s="76" t="s">
+      <c r="F32" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="76" t="s">
+      <c r="G32" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3940,10 +4044,10 @@
       <c r="E33" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="76" t="s">
+      <c r="F33" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="76" t="s">
+      <c r="G33" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3963,10 +4067,10 @@
       <c r="E34" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="76" t="s">
+      <c r="F34" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="76" t="s">
+      <c r="G34" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3986,10 +4090,10 @@
       <c r="E35" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="76" t="s">
+      <c r="F35" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="76" t="s">
+      <c r="G35" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4009,10 +4113,10 @@
       <c r="E36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="76" t="s">
+      <c r="F36" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="76" t="s">
+      <c r="G36" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4032,10 +4136,10 @@
       <c r="E37" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="76" t="s">
+      <c r="F37" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G37" s="76" t="s">
+      <c r="G37" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4055,10 +4159,10 @@
       <c r="E38" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="76" t="s">
+      <c r="F38" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="76" t="s">
+      <c r="G38" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4078,10 +4182,10 @@
       <c r="E39" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="76" t="s">
+      <c r="F39" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="76" t="s">
+      <c r="G39" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4101,10 +4205,10 @@
       <c r="E40" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="76" t="s">
+      <c r="F40" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="76" t="s">
+      <c r="G40" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4124,10 +4228,10 @@
       <c r="E41" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="76" t="s">
+      <c r="F41" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="76" t="s">
+      <c r="G41" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4147,10 +4251,10 @@
       <c r="E42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="76" t="s">
+      <c r="F42" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="76" t="s">
+      <c r="G42" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4170,10 +4274,10 @@
       <c r="E43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F43" s="76" t="s">
+      <c r="F43" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="76" t="s">
+      <c r="G43" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4193,10 +4297,10 @@
       <c r="E44" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="F44" s="76" t="s">
+      <c r="F44" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="76" t="s">
+      <c r="G44" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4216,10 +4320,10 @@
       <c r="E45" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F45" s="76" t="s">
+      <c r="F45" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="76" t="s">
+      <c r="G45" s="75" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4239,10 +4343,10 @@
       <c r="E46" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="76" t="s">
+      <c r="F46" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G46" s="76" t="s">
+      <c r="G46" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4262,10 +4366,10 @@
       <c r="E47" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="76" t="s">
+      <c r="F47" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="76" t="s">
+      <c r="G47" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4285,10 +4389,10 @@
       <c r="E48" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="76" t="s">
+      <c r="F48" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G48" s="76" t="s">
+      <c r="G48" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4308,10 +4412,10 @@
       <c r="E49" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="76" t="s">
+      <c r="F49" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G49" s="76" t="s">
+      <c r="G49" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4331,10 +4435,10 @@
       <c r="E50" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="76" t="s">
+      <c r="F50" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G50" s="76" t="s">
+      <c r="G50" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4354,10 +4458,10 @@
       <c r="E51" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F51" s="76" t="s">
+      <c r="F51" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G51" s="76" t="s">
+      <c r="G51" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4377,10 +4481,10 @@
       <c r="E52" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F52" s="76" t="s">
+      <c r="F52" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G52" s="76" t="s">
+      <c r="G52" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4400,10 +4504,10 @@
       <c r="E53" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F53" s="76" t="s">
+      <c r="F53" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="76" t="s">
+      <c r="G53" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4423,10 +4527,10 @@
       <c r="E54" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="76" t="s">
+      <c r="F54" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="76" t="s">
+      <c r="G54" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4446,10 +4550,10 @@
       <c r="E55" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F55" s="76" t="s">
+      <c r="F55" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="76" t="s">
+      <c r="G55" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4469,10 +4573,10 @@
       <c r="E56" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F56" s="76" t="s">
+      <c r="F56" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="76" t="s">
+      <c r="G56" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4492,10 +4596,10 @@
       <c r="E57" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F57" s="76" t="s">
+      <c r="F57" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G57" s="76" t="s">
+      <c r="G57" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4515,10 +4619,10 @@
       <c r="E58" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F58" s="76" t="s">
+      <c r="F58" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G58" s="76" t="s">
+      <c r="G58" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4538,10 +4642,10 @@
       <c r="E59" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="76" t="s">
+      <c r="F59" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="76" t="s">
+      <c r="G59" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4561,10 +4665,10 @@
       <c r="E60" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F60" s="76" t="s">
+      <c r="F60" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="76" t="s">
+      <c r="G60" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4584,10 +4688,10 @@
       <c r="E61" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F61" s="76" t="s">
+      <c r="F61" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G61" s="76" t="s">
+      <c r="G61" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4607,10 +4711,10 @@
       <c r="E62" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="76" t="s">
+      <c r="F62" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G62" s="76" t="s">
+      <c r="G62" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4630,10 +4734,10 @@
       <c r="E63" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F63" s="76" t="s">
+      <c r="F63" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G63" s="76" t="s">
+      <c r="G63" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4653,10 +4757,10 @@
       <c r="E64" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="76" t="s">
+      <c r="F64" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="76" t="s">
+      <c r="G64" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4676,10 +4780,10 @@
       <c r="E65" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="76" t="s">
+      <c r="F65" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G65" s="76" t="s">
+      <c r="G65" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4699,10 +4803,10 @@
       <c r="E66" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="76" t="s">
+      <c r="F66" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G66" s="76" t="s">
+      <c r="G66" s="75" t="s">
         <v>12</v>
       </c>
     </row>
@@ -4722,10 +4826,10 @@
       <c r="E67" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="76" t="s">
+      <c r="F67" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G67" s="76" t="s">
+      <c r="G67" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4745,10 +4849,10 @@
       <c r="E68" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="76" t="s">
+      <c r="F68" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G68" s="76" t="s">
+      <c r="G68" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4768,10 +4872,10 @@
       <c r="E69" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F69" s="76" t="s">
+      <c r="F69" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G69" s="76" t="s">
+      <c r="G69" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4791,10 +4895,10 @@
       <c r="E70" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F70" s="76" t="s">
+      <c r="F70" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G70" s="76" t="s">
+      <c r="G70" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4814,10 +4918,10 @@
       <c r="E71" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="76" t="s">
+      <c r="F71" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G71" s="76" t="s">
+      <c r="G71" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4837,10 +4941,10 @@
       <c r="E72" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="76" t="s">
+      <c r="F72" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G72" s="76" t="s">
+      <c r="G72" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4860,10 +4964,10 @@
       <c r="E73" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F73" s="76" t="s">
+      <c r="F73" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G73" s="76" t="s">
+      <c r="G73" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4883,10 +4987,10 @@
       <c r="E74" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F74" s="76" t="s">
+      <c r="F74" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G74" s="76" t="s">
+      <c r="G74" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4906,10 +5010,10 @@
       <c r="E75" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F75" s="76" t="s">
+      <c r="F75" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G75" s="76" t="s">
+      <c r="G75" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4929,10 +5033,10 @@
       <c r="E76" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="76" t="s">
+      <c r="F76" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G76" s="76" t="s">
+      <c r="G76" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4952,10 +5056,10 @@
       <c r="E77" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="76" t="s">
+      <c r="F77" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G77" s="76" t="s">
+      <c r="G77" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4975,10 +5079,10 @@
       <c r="E78" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="76" t="s">
+      <c r="F78" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G78" s="76" t="s">
+      <c r="G78" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4998,10 +5102,10 @@
       <c r="E79" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F79" s="76" t="s">
+      <c r="F79" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G79" s="76" t="s">
+      <c r="G79" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5021,10 +5125,10 @@
       <c r="E80" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="F80" s="76" t="s">
+      <c r="F80" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="G80" s="76" t="s">
+      <c r="G80" s="75" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5044,10 +5148,10 @@
       <c r="E81" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F81" s="76" t="s">
+      <c r="F81" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G81" s="76" t="s">
+      <c r="G81" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5067,10 +5171,10 @@
       <c r="E82" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F82" s="76" t="s">
+      <c r="F82" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G82" s="76" t="s">
+      <c r="G82" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5090,10 +5194,10 @@
       <c r="E83" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="76" t="s">
+      <c r="F83" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G83" s="76" t="s">
+      <c r="G83" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5113,10 +5217,10 @@
       <c r="E84" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F84" s="76" t="s">
+      <c r="F84" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G84" s="76" t="s">
+      <c r="G84" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5136,10 +5240,10 @@
       <c r="E85" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F85" s="76" t="s">
+      <c r="F85" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G85" s="76" t="s">
+      <c r="G85" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5159,10 +5263,10 @@
       <c r="E86" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="76" t="s">
+      <c r="F86" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G86" s="76" t="s">
+      <c r="G86" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5182,10 +5286,10 @@
       <c r="E87" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="76" t="s">
+      <c r="F87" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G87" s="76" t="s">
+      <c r="G87" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5205,10 +5309,10 @@
       <c r="E88" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F88" s="76" t="s">
+      <c r="F88" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G88" s="76" t="s">
+      <c r="G88" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5228,10 +5332,10 @@
       <c r="E89" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="76" t="s">
+      <c r="F89" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G89" s="76" t="s">
+      <c r="G89" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5251,10 +5355,10 @@
       <c r="E90" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F90" s="76" t="s">
+      <c r="F90" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G90" s="76" t="s">
+      <c r="G90" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5274,10 +5378,10 @@
       <c r="E91" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="76" t="s">
+      <c r="F91" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G91" s="76" t="s">
+      <c r="G91" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5297,10 +5401,10 @@
       <c r="E92" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="76" t="s">
+      <c r="F92" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G92" s="76" t="s">
+      <c r="G92" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5320,10 +5424,10 @@
       <c r="E93" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="76" t="s">
+      <c r="F93" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G93" s="76" t="s">
+      <c r="G93" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5343,10 +5447,10 @@
       <c r="E94" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F94" s="76" t="s">
+      <c r="F94" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G94" s="76" t="s">
+      <c r="G94" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5366,10 +5470,10 @@
       <c r="E95" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="76" t="s">
+      <c r="F95" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G95" s="76" t="s">
+      <c r="G95" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5389,10 +5493,10 @@
       <c r="E96" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="76" t="s">
+      <c r="F96" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G96" s="76" t="s">
+      <c r="G96" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5412,10 +5516,10 @@
       <c r="E97" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F97" s="76" t="s">
+      <c r="F97" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G97" s="76" t="s">
+      <c r="G97" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5435,10 +5539,10 @@
       <c r="E98" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F98" s="76" t="s">
+      <c r="F98" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G98" s="76" t="s">
+      <c r="G98" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5458,10 +5562,10 @@
       <c r="E99" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="76" t="s">
+      <c r="F99" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G99" s="76" t="s">
+      <c r="G99" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5481,10 +5585,10 @@
       <c r="E100" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F100" s="76" t="s">
+      <c r="F100" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G100" s="76" t="s">
+      <c r="G100" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5504,10 +5608,10 @@
       <c r="E101" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F101" s="76" t="s">
+      <c r="F101" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G101" s="76" t="s">
+      <c r="G101" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5527,10 +5631,10 @@
       <c r="E102" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F102" s="76" t="s">
+      <c r="F102" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G102" s="76" t="s">
+      <c r="G102" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5550,10 +5654,10 @@
       <c r="E103" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F103" s="76" t="s">
+      <c r="F103" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G103" s="76" t="s">
+      <c r="G103" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5573,10 +5677,10 @@
       <c r="E104" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F104" s="76" t="s">
+      <c r="F104" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G104" s="76" t="s">
+      <c r="G104" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5596,10 +5700,10 @@
       <c r="E105" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F105" s="76" t="s">
+      <c r="F105" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G105" s="76" t="s">
+      <c r="G105" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5619,10 +5723,10 @@
       <c r="E106" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F106" s="76" t="s">
+      <c r="F106" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G106" s="76" t="s">
+      <c r="G106" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5642,10 +5746,10 @@
       <c r="E107" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F107" s="76" t="s">
+      <c r="F107" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G107" s="76" t="s">
+      <c r="G107" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5665,10 +5769,10 @@
       <c r="E108" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F108" s="76" t="s">
+      <c r="F108" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G108" s="76" t="s">
+      <c r="G108" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5688,10 +5792,10 @@
       <c r="E109" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F109" s="76" t="s">
+      <c r="F109" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G109" s="76" t="s">
+      <c r="G109" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5711,10 +5815,10 @@
       <c r="E110" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F110" s="76" t="s">
+      <c r="F110" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G110" s="76" t="s">
+      <c r="G110" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5734,10 +5838,10 @@
       <c r="E111" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F111" s="76" t="s">
+      <c r="F111" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G111" s="76" t="s">
+      <c r="G111" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5757,10 +5861,10 @@
       <c r="E112" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F112" s="76" t="s">
+      <c r="F112" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G112" s="76" t="s">
+      <c r="G112" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5780,10 +5884,10 @@
       <c r="E113" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F113" s="76" t="s">
+      <c r="F113" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G113" s="76" t="s">
+      <c r="G113" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5803,10 +5907,10 @@
       <c r="E114" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F114" s="76" t="s">
+      <c r="F114" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G114" s="76" t="s">
+      <c r="G114" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5826,10 +5930,10 @@
       <c r="E115" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F115" s="76" t="s">
+      <c r="F115" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G115" s="76" t="s">
+      <c r="G115" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5849,10 +5953,10 @@
       <c r="E116" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F116" s="76" t="s">
+      <c r="F116" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G116" s="76" t="s">
+      <c r="G116" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5872,10 +5976,10 @@
       <c r="E117" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F117" s="76" t="s">
+      <c r="F117" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G117" s="76" t="s">
+      <c r="G117" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5895,10 +5999,10 @@
       <c r="E118" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F118" s="76" t="s">
+      <c r="F118" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G118" s="76" t="s">
+      <c r="G118" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5918,10 +6022,10 @@
       <c r="E119" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F119" s="76" t="s">
+      <c r="F119" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G119" s="76" t="s">
+      <c r="G119" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5941,10 +6045,10 @@
       <c r="E120" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F120" s="76" t="s">
+      <c r="F120" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G120" s="76" t="s">
+      <c r="G120" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5964,10 +6068,10 @@
       <c r="E121" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F121" s="76" t="s">
+      <c r="F121" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G121" s="76" t="s">
+      <c r="G121" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5987,10 +6091,10 @@
       <c r="E122" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F122" s="76" t="s">
+      <c r="F122" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G122" s="76" t="s">
+      <c r="G122" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6010,10 +6114,10 @@
       <c r="E123" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F123" s="76" t="s">
+      <c r="F123" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G123" s="76" t="s">
+      <c r="G123" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6033,10 +6137,10 @@
       <c r="E124" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F124" s="76" t="s">
+      <c r="F124" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G124" s="76" t="s">
+      <c r="G124" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6056,10 +6160,10 @@
       <c r="E125" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F125" s="76" t="s">
+      <c r="F125" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G125" s="76" t="s">
+      <c r="G125" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6079,10 +6183,10 @@
       <c r="E126" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F126" s="76" t="s">
+      <c r="F126" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G126" s="76" t="s">
+      <c r="G126" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6102,10 +6206,10 @@
       <c r="E127" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F127" s="76" t="s">
+      <c r="F127" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G127" s="76" t="s">
+      <c r="G127" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6125,10 +6229,10 @@
       <c r="E128" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F128" s="76" t="s">
+      <c r="F128" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G128" s="76" t="s">
+      <c r="G128" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6148,10 +6252,10 @@
       <c r="E129" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F129" s="76" t="s">
+      <c r="F129" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G129" s="76" t="s">
+      <c r="G129" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6171,10 +6275,10 @@
       <c r="E130" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F130" s="76" t="s">
+      <c r="F130" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G130" s="76" t="s">
+      <c r="G130" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6194,10 +6298,10 @@
       <c r="E131" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="F131" s="76" t="s">
+      <c r="F131" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="G131" s="76" t="s">
+      <c r="G131" s="75" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6217,10 +6321,10 @@
       <c r="E132" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F132" s="76" t="s">
+      <c r="F132" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G132" s="76" t="s">
+      <c r="G132" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6240,10 +6344,10 @@
       <c r="E133" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F133" s="76" t="s">
+      <c r="F133" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G133" s="76" t="s">
+      <c r="G133" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6263,10 +6367,10 @@
       <c r="E134" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F134" s="76" t="s">
+      <c r="F134" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G134" s="76" t="s">
+      <c r="G134" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6286,10 +6390,10 @@
       <c r="E135" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F135" s="76" t="s">
+      <c r="F135" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G135" s="76" t="s">
+      <c r="G135" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6309,10 +6413,10 @@
       <c r="E136" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F136" s="76" t="s">
+      <c r="F136" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G136" s="76" t="s">
+      <c r="G136" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6332,10 +6436,10 @@
       <c r="E137" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F137" s="76" t="s">
+      <c r="F137" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G137" s="76" t="s">
+      <c r="G137" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6355,10 +6459,10 @@
       <c r="E138" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F138" s="76" t="s">
+      <c r="F138" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G138" s="76" t="s">
+      <c r="G138" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6378,10 +6482,10 @@
       <c r="E139" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F139" s="76" t="s">
+      <c r="F139" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G139" s="76" t="s">
+      <c r="G139" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6401,10 +6505,10 @@
       <c r="E140" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F140" s="76" t="s">
+      <c r="F140" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G140" s="76" t="s">
+      <c r="G140" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6424,10 +6528,10 @@
       <c r="E141" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F141" s="76" t="s">
+      <c r="F141" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G141" s="76" t="s">
+      <c r="G141" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6447,10 +6551,10 @@
       <c r="E142" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F142" s="76" t="s">
+      <c r="F142" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G142" s="76" t="s">
+      <c r="G142" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6470,10 +6574,10 @@
       <c r="E143" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F143" s="76" t="s">
+      <c r="F143" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G143" s="76" t="s">
+      <c r="G143" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6493,10 +6597,10 @@
       <c r="E144" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F144" s="76" t="s">
+      <c r="F144" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G144" s="76" t="s">
+      <c r="G144" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6516,10 +6620,10 @@
       <c r="E145" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F145" s="76" t="s">
+      <c r="F145" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G145" s="76" t="s">
+      <c r="G145" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6539,10 +6643,10 @@
       <c r="E146" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F146" s="76" t="s">
+      <c r="F146" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G146" s="76" t="s">
+      <c r="G146" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6562,10 +6666,10 @@
       <c r="E147" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F147" s="76" t="s">
+      <c r="F147" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G147" s="76" t="s">
+      <c r="G147" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6585,10 +6689,10 @@
       <c r="E148" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F148" s="76" t="s">
+      <c r="F148" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G148" s="76" t="s">
+      <c r="G148" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6608,10 +6712,10 @@
       <c r="E149" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F149" s="76" t="s">
+      <c r="F149" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G149" s="76" t="s">
+      <c r="G149" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6631,10 +6735,10 @@
       <c r="E150" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F150" s="76" t="s">
+      <c r="F150" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G150" s="76" t="s">
+      <c r="G150" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6654,10 +6758,10 @@
       <c r="E151" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F151" s="76" t="s">
+      <c r="F151" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G151" s="76" t="s">
+      <c r="G151" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6677,10 +6781,10 @@
       <c r="E152" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F152" s="76" t="s">
+      <c r="F152" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G152" s="76" t="s">
+      <c r="G152" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6700,10 +6804,10 @@
       <c r="E153" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F153" s="76" t="s">
+      <c r="F153" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G153" s="76" t="s">
+      <c r="G153" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6723,10 +6827,10 @@
       <c r="E154" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F154" s="76" t="s">
+      <c r="F154" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G154" s="76" t="s">
+      <c r="G154" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6746,10 +6850,10 @@
       <c r="E155" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F155" s="76" t="s">
+      <c r="F155" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G155" s="76" t="s">
+      <c r="G155" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6769,10 +6873,10 @@
       <c r="E156" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F156" s="76" t="s">
+      <c r="F156" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G156" s="76" t="s">
+      <c r="G156" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6792,10 +6896,10 @@
       <c r="E157" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F157" s="76" t="s">
+      <c r="F157" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G157" s="76" t="s">
+      <c r="G157" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6815,10 +6919,10 @@
       <c r="E158" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F158" s="76" t="s">
+      <c r="F158" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G158" s="76" t="s">
+      <c r="G158" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6838,10 +6942,10 @@
       <c r="E159" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="F159" s="76" t="s">
+      <c r="F159" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="G159" s="76" t="s">
+      <c r="G159" s="75" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6861,10 +6965,10 @@
       <c r="E160" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F160" s="76" t="s">
+      <c r="F160" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G160" s="76" t="s">
+      <c r="G160" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6884,10 +6988,10 @@
       <c r="E161" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F161" s="76" t="s">
+      <c r="F161" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G161" s="76" t="s">
+      <c r="G161" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6907,10 +7011,10 @@
       <c r="E162" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F162" s="76" t="s">
+      <c r="F162" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G162" s="76" t="s">
+      <c r="G162" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6930,10 +7034,10 @@
       <c r="E163" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F163" s="76" t="s">
+      <c r="F163" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G163" s="76" t="s">
+      <c r="G163" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6953,10 +7057,10 @@
       <c r="E164" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F164" s="76" t="s">
+      <c r="F164" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G164" s="76" t="s">
+      <c r="G164" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6976,10 +7080,10 @@
       <c r="E165" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F165" s="76" t="s">
+      <c r="F165" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G165" s="76" t="s">
+      <c r="G165" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -6999,10 +7103,10 @@
       <c r="E166" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F166" s="76" t="s">
+      <c r="F166" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G166" s="76" t="s">
+      <c r="G166" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7022,10 +7126,10 @@
       <c r="E167" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F167" s="76" t="s">
+      <c r="F167" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G167" s="76" t="s">
+      <c r="G167" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7045,10 +7149,10 @@
       <c r="E168" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F168" s="76" t="s">
+      <c r="F168" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G168" s="76" t="s">
+      <c r="G168" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7068,10 +7172,10 @@
       <c r="E169" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F169" s="76" t="s">
+      <c r="F169" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G169" s="76" t="s">
+      <c r="G169" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7091,10 +7195,10 @@
       <c r="E170" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F170" s="76" t="s">
+      <c r="F170" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G170" s="76" t="s">
+      <c r="G170" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7114,10 +7218,10 @@
       <c r="E171" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F171" s="76" t="s">
+      <c r="F171" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G171" s="76" t="s">
+      <c r="G171" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7137,10 +7241,10 @@
       <c r="E172" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F172" s="76" t="s">
+      <c r="F172" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G172" s="76" t="s">
+      <c r="G172" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7160,10 +7264,10 @@
       <c r="E173" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F173" s="76" t="s">
+      <c r="F173" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G173" s="76" t="s">
+      <c r="G173" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7183,10 +7287,10 @@
       <c r="E174" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F174" s="76" t="s">
+      <c r="F174" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G174" s="76" t="s">
+      <c r="G174" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7206,10 +7310,10 @@
       <c r="E175" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F175" s="76" t="s">
+      <c r="F175" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G175" s="76" t="s">
+      <c r="G175" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7229,10 +7333,10 @@
       <c r="E176" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F176" s="76" t="s">
+      <c r="F176" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G176" s="76" t="s">
+      <c r="G176" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7252,10 +7356,10 @@
       <c r="E177" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F177" s="76" t="s">
+      <c r="F177" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G177" s="76" t="s">
+      <c r="G177" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7275,10 +7379,10 @@
       <c r="E178" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F178" s="76" t="s">
+      <c r="F178" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G178" s="76" t="s">
+      <c r="G178" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7298,10 +7402,10 @@
       <c r="E179" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F179" s="76" t="s">
+      <c r="F179" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G179" s="76" t="s">
+      <c r="G179" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7321,10 +7425,10 @@
       <c r="E180" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F180" s="76" t="s">
+      <c r="F180" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G180" s="76" t="s">
+      <c r="G180" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7344,10 +7448,10 @@
       <c r="E181" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F181" s="76" t="s">
+      <c r="F181" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G181" s="76" t="s">
+      <c r="G181" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7367,10 +7471,10 @@
       <c r="E182" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F182" s="76" t="s">
+      <c r="F182" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G182" s="76" t="s">
+      <c r="G182" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7390,10 +7494,10 @@
       <c r="E183" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F183" s="76" t="s">
+      <c r="F183" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G183" s="76" t="s">
+      <c r="G183" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7413,10 +7517,10 @@
       <c r="E184" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F184" s="76" t="s">
+      <c r="F184" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G184" s="76" t="s">
+      <c r="G184" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7436,10 +7540,10 @@
       <c r="E185" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F185" s="76" t="s">
+      <c r="F185" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G185" s="76" t="s">
+      <c r="G185" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7459,10 +7563,10 @@
       <c r="E186" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F186" s="76" t="s">
+      <c r="F186" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G186" s="76" t="s">
+      <c r="G186" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7482,10 +7586,10 @@
       <c r="E187" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F187" s="76" t="s">
+      <c r="F187" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G187" s="76" t="s">
+      <c r="G187" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7505,10 +7609,10 @@
       <c r="E188" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F188" s="76" t="s">
+      <c r="F188" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G188" s="76" t="s">
+      <c r="G188" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7528,10 +7632,10 @@
       <c r="E189" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F189" s="76" t="s">
+      <c r="F189" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G189" s="76" t="s">
+      <c r="G189" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7551,10 +7655,10 @@
       <c r="E190" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F190" s="76" t="s">
+      <c r="F190" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G190" s="76" t="s">
+      <c r="G190" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7574,10 +7678,10 @@
       <c r="E191" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F191" s="76" t="s">
+      <c r="F191" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G191" s="76" t="s">
+      <c r="G191" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7597,10 +7701,10 @@
       <c r="E192" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F192" s="76" t="s">
+      <c r="F192" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G192" s="76" t="s">
+      <c r="G192" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7620,10 +7724,10 @@
       <c r="E193" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F193" s="76" t="s">
+      <c r="F193" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G193" s="76" t="s">
+      <c r="G193" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7643,10 +7747,10 @@
       <c r="E194" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F194" s="76" t="s">
+      <c r="F194" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G194" s="76" t="s">
+      <c r="G194" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7666,10 +7770,10 @@
       <c r="E195" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F195" s="76" t="s">
+      <c r="F195" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G195" s="76" t="s">
+      <c r="G195" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7689,10 +7793,10 @@
       <c r="E196" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F196" s="76" t="s">
+      <c r="F196" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G196" s="76" t="s">
+      <c r="G196" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7712,10 +7816,10 @@
       <c r="E197" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F197" s="76" t="s">
+      <c r="F197" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G197" s="76" t="s">
+      <c r="G197" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7735,10 +7839,10 @@
       <c r="E198" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F198" s="76" t="s">
+      <c r="F198" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G198" s="76" t="s">
+      <c r="G198" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7758,10 +7862,10 @@
       <c r="E199" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F199" s="76" t="s">
+      <c r="F199" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G199" s="76" t="s">
+      <c r="G199" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7781,10 +7885,10 @@
       <c r="E200" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F200" s="76" t="s">
+      <c r="F200" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G200" s="76" t="s">
+      <c r="G200" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7804,10 +7908,10 @@
       <c r="E201" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F201" s="76" t="s">
+      <c r="F201" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G201" s="76" t="s">
+      <c r="G201" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7827,10 +7931,10 @@
       <c r="E202" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F202" s="76" t="s">
+      <c r="F202" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G202" s="76" t="s">
+      <c r="G202" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7850,10 +7954,10 @@
       <c r="E203" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F203" s="76" t="s">
+      <c r="F203" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G203" s="76" t="s">
+      <c r="G203" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7873,10 +7977,10 @@
       <c r="E204" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F204" s="76" t="s">
+      <c r="F204" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G204" s="76" t="s">
+      <c r="G204" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7896,10 +8000,10 @@
       <c r="E205" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F205" s="76" t="s">
+      <c r="F205" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G205" s="76" t="s">
+      <c r="G205" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7919,10 +8023,10 @@
       <c r="E206" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F206" s="76" t="s">
+      <c r="F206" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G206" s="76" t="s">
+      <c r="G206" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7942,10 +8046,10 @@
       <c r="E207" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F207" s="76" t="s">
+      <c r="F207" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G207" s="76" t="s">
+      <c r="G207" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7965,10 +8069,10 @@
       <c r="E208" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F208" s="76" t="s">
+      <c r="F208" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G208" s="76" t="s">
+      <c r="G208" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -7988,10 +8092,10 @@
       <c r="E209" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F209" s="76" t="s">
+      <c r="F209" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G209" s="76" t="s">
+      <c r="G209" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8011,10 +8115,10 @@
       <c r="E210" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F210" s="76" t="s">
+      <c r="F210" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G210" s="76" t="s">
+      <c r="G210" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8034,10 +8138,10 @@
       <c r="E211" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F211" s="76" t="s">
+      <c r="F211" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G211" s="76" t="s">
+      <c r="G211" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8057,10 +8161,10 @@
       <c r="E212" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F212" s="76" t="s">
+      <c r="F212" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G212" s="76" t="s">
+      <c r="G212" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8080,10 +8184,10 @@
       <c r="E213" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F213" s="76" t="s">
+      <c r="F213" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G213" s="76" t="s">
+      <c r="G213" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8103,10 +8207,10 @@
       <c r="E214" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F214" s="76" t="s">
+      <c r="F214" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G214" s="76" t="s">
+      <c r="G214" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8126,10 +8230,10 @@
       <c r="E215" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F215" s="76" t="s">
+      <c r="F215" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G215" s="76" t="s">
+      <c r="G215" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8149,10 +8253,10 @@
       <c r="E216" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F216" s="76" t="s">
+      <c r="F216" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G216" s="76" t="s">
+      <c r="G216" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8172,10 +8276,10 @@
       <c r="E217" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F217" s="76" t="s">
+      <c r="F217" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G217" s="76" t="s">
+      <c r="G217" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8195,10 +8299,10 @@
       <c r="E218" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F218" s="76" t="s">
+      <c r="F218" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G218" s="76" t="s">
+      <c r="G218" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8218,10 +8322,10 @@
       <c r="E219" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F219" s="76" t="s">
+      <c r="F219" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G219" s="76" t="s">
+      <c r="G219" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8241,10 +8345,10 @@
       <c r="E220" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F220" s="76" t="s">
+      <c r="F220" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G220" s="76" t="s">
+      <c r="G220" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8264,10 +8368,10 @@
       <c r="E221" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F221" s="76" t="s">
+      <c r="F221" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G221" s="76" t="s">
+      <c r="G221" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8287,10 +8391,10 @@
       <c r="E222" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F222" s="76" t="s">
+      <c r="F222" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G222" s="76" t="s">
+      <c r="G222" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8310,10 +8414,10 @@
       <c r="E223" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F223" s="76" t="s">
+      <c r="F223" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G223" s="76" t="s">
+      <c r="G223" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8333,10 +8437,10 @@
       <c r="E224" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F224" s="76" t="s">
+      <c r="F224" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G224" s="76" t="s">
+      <c r="G224" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8356,10 +8460,10 @@
       <c r="E225" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F225" s="76" t="s">
+      <c r="F225" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G225" s="76" t="s">
+      <c r="G225" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8379,10 +8483,10 @@
       <c r="E226" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F226" s="76" t="s">
+      <c r="F226" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G226" s="76" t="s">
+      <c r="G226" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8402,10 +8506,10 @@
       <c r="E227" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F227" s="76" t="s">
+      <c r="F227" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G227" s="76" t="s">
+      <c r="G227" s="75" t="s">
         <v>22</v>
       </c>
     </row>
@@ -8425,217 +8529,217 @@
       <c r="E228" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F228" s="76" t="s">
+      <c r="F228" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="G228" s="76" t="s">
+      <c r="G228" s="75" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="229" spans="1:7">
-      <c r="A229" s="79">
+      <c r="A229" s="78">
         <v>3</v>
       </c>
-      <c r="B229" s="79">
-        <v>0</v>
-      </c>
-      <c r="C229" s="79">
-        <v>0</v>
-      </c>
-      <c r="D229" s="79">
-        <v>0</v>
-      </c>
-      <c r="E229" s="79" t="s">
+      <c r="B229" s="78">
+        <v>0</v>
+      </c>
+      <c r="C229" s="78">
+        <v>0</v>
+      </c>
+      <c r="D229" s="78">
+        <v>0</v>
+      </c>
+      <c r="E229" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F229" s="76" t="s">
+      <c r="F229" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G229" s="76" t="s">
+      <c r="G229" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="230" spans="1:7">
-      <c r="A230" s="79">
+      <c r="A230" s="78">
         <v>3</v>
       </c>
-      <c r="B230" s="79">
+      <c r="B230" s="78">
         <v>20</v>
       </c>
-      <c r="C230" s="79">
-        <v>0</v>
-      </c>
-      <c r="D230" s="79">
+      <c r="C230" s="78">
+        <v>0</v>
+      </c>
+      <c r="D230" s="78">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E230" s="79" t="s">
+      <c r="E230" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F230" s="76" t="s">
+      <c r="F230" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G230" s="76" t="s">
+      <c r="G230" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="231" spans="1:7">
-      <c r="A231" s="79">
+      <c r="A231" s="78">
         <v>3</v>
       </c>
-      <c r="B231" s="79">
+      <c r="B231" s="78">
         <v>30</v>
       </c>
-      <c r="C231" s="79">
-        <v>0</v>
-      </c>
-      <c r="D231" s="79">
-        <v>0</v>
-      </c>
-      <c r="E231" s="79" t="s">
+      <c r="C231" s="78">
+        <v>0</v>
+      </c>
+      <c r="D231" s="78">
+        <v>0</v>
+      </c>
+      <c r="E231" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F231" s="76" t="s">
+      <c r="F231" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G231" s="76" t="s">
+      <c r="G231" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="232" spans="1:7">
-      <c r="A232" s="79">
+      <c r="A232" s="78">
         <v>3</v>
       </c>
-      <c r="B232" s="79">
+      <c r="B232" s="78">
         <v>40</v>
       </c>
-      <c r="C232" s="79">
+      <c r="C232" s="78">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="D232" s="79">
+      <c r="D232" s="78">
         <v>0.16</v>
       </c>
-      <c r="E232" s="79" t="s">
+      <c r="E232" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F232" s="76" t="s">
+      <c r="F232" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G232" s="76" t="s">
+      <c r="G232" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="233" spans="1:7">
-      <c r="A233" s="79">
+      <c r="A233" s="78">
         <v>3</v>
       </c>
-      <c r="B233" s="79">
+      <c r="B233" s="78">
         <v>50</v>
       </c>
-      <c r="C233" s="79">
+      <c r="C233" s="78">
         <v>5.4054054054054057E-2</v>
       </c>
-      <c r="D233" s="79">
+      <c r="D233" s="78">
         <v>0.37</v>
       </c>
-      <c r="E233" s="79" t="s">
+      <c r="E233" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F233" s="76" t="s">
+      <c r="F233" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G233" s="76" t="s">
+      <c r="G233" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="234" spans="1:7">
-      <c r="A234" s="79">
+      <c r="A234" s="78">
         <v>3</v>
       </c>
-      <c r="B234" s="79">
+      <c r="B234" s="78">
         <v>60</v>
       </c>
-      <c r="C234" s="79">
+      <c r="C234" s="78">
         <v>0.10461538461538462</v>
       </c>
-      <c r="D234" s="79">
+      <c r="D234" s="78">
         <v>0.65</v>
       </c>
-      <c r="E234" s="79" t="s">
+      <c r="E234" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F234" s="76" t="s">
+      <c r="F234" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G234" s="76" t="s">
+      <c r="G234" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="235" spans="1:7">
-      <c r="A235" s="79">
+      <c r="A235" s="78">
         <v>3</v>
       </c>
-      <c r="B235" s="79">
+      <c r="B235" s="78">
         <v>70</v>
       </c>
-      <c r="C235" s="79">
+      <c r="C235" s="78">
         <v>0.21176470588235294</v>
       </c>
-      <c r="D235" s="79">
+      <c r="D235" s="78">
         <v>0.85</v>
       </c>
-      <c r="E235" s="79" t="s">
+      <c r="E235" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F235" s="76" t="s">
+      <c r="F235" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G235" s="76" t="s">
+      <c r="G235" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="236" spans="1:7">
-      <c r="A236" s="79">
+      <c r="A236" s="78">
         <v>3</v>
       </c>
-      <c r="B236" s="79">
+      <c r="B236" s="78">
         <v>80</v>
       </c>
-      <c r="C236" s="79">
+      <c r="C236" s="78">
         <v>0.4</v>
       </c>
-      <c r="D236" s="79">
-        <v>1</v>
-      </c>
-      <c r="E236" s="79" t="s">
+      <c r="D236" s="78">
+        <v>1</v>
+      </c>
+      <c r="E236" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F236" s="76" t="s">
+      <c r="F236" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G236" s="76" t="s">
+      <c r="G236" s="75" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="237" spans="1:7">
-      <c r="A237" s="79">
+      <c r="A237" s="78">
         <v>3</v>
       </c>
-      <c r="B237" s="79">
+      <c r="B237" s="78">
         <v>100</v>
       </c>
-      <c r="C237" s="79">
+      <c r="C237" s="78">
         <v>0.4</v>
       </c>
-      <c r="D237" s="79">
-        <v>1</v>
-      </c>
-      <c r="E237" s="79" t="s">
+      <c r="D237" s="78">
+        <v>1</v>
+      </c>
+      <c r="E237" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="F237" s="76" t="s">
+      <c r="F237" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G237" s="76" t="s">
+      <c r="G237" s="75" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8655,10 +8759,10 @@
       <c r="E238" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F238" s="76" t="s">
+      <c r="F238" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G238" s="76" t="s">
+      <c r="G238" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8678,10 +8782,10 @@
       <c r="E239" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F239" s="76" t="s">
+      <c r="F239" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G239" s="76" t="s">
+      <c r="G239" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8701,10 +8805,10 @@
       <c r="E240" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F240" s="76" t="s">
+      <c r="F240" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G240" s="76" t="s">
+      <c r="G240" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8724,10 +8828,10 @@
       <c r="E241" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F241" s="76" t="s">
+      <c r="F241" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G241" s="76" t="s">
+      <c r="G241" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8747,10 +8851,10 @@
       <c r="E242" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F242" s="76" t="s">
+      <c r="F242" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G242" s="76" t="s">
+      <c r="G242" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8770,10 +8874,10 @@
       <c r="E243" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F243" s="76" t="s">
+      <c r="F243" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G243" s="76" t="s">
+      <c r="G243" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8793,10 +8897,10 @@
       <c r="E244" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F244" s="76" t="s">
+      <c r="F244" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G244" s="76" t="s">
+      <c r="G244" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8816,10 +8920,10 @@
       <c r="E245" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F245" s="76" t="s">
+      <c r="F245" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G245" s="76" t="s">
+      <c r="G245" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8839,10 +8943,10 @@
       <c r="E246" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F246" s="76" t="s">
+      <c r="F246" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G246" s="76" t="s">
+      <c r="G246" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8862,10 +8966,10 @@
       <c r="E247" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F247" s="76" t="s">
+      <c r="F247" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G247" s="76" t="s">
+      <c r="G247" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8885,10 +8989,10 @@
       <c r="E248" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F248" s="76" t="s">
+      <c r="F248" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G248" s="76" t="s">
+      <c r="G248" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8908,10 +9012,10 @@
       <c r="E249" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F249" s="76" t="s">
+      <c r="F249" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G249" s="76" t="s">
+      <c r="G249" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8931,10 +9035,10 @@
       <c r="E250" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F250" s="76" t="s">
+      <c r="F250" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G250" s="76" t="s">
+      <c r="G250" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8954,10 +9058,10 @@
       <c r="E251" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F251" s="76" t="s">
+      <c r="F251" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G251" s="76" t="s">
+      <c r="G251" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -8977,10 +9081,10 @@
       <c r="E252" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F252" s="76" t="s">
+      <c r="F252" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G252" s="76" t="s">
+      <c r="G252" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -9000,10 +9104,10 @@
       <c r="E253" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F253" s="76" t="s">
+      <c r="F253" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G253" s="76" t="s">
+      <c r="G253" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -9023,10 +9127,10 @@
       <c r="E254" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F254" s="76" t="s">
+      <c r="F254" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G254" s="76" t="s">
+      <c r="G254" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -9046,10 +9150,10 @@
       <c r="E255" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F255" s="76" t="s">
+      <c r="F255" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G255" s="76" t="s">
+      <c r="G255" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -9069,10 +9173,10 @@
       <c r="E256" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="F256" s="76" t="s">
+      <c r="F256" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="G256" s="76" t="s">
+      <c r="G256" s="75" t="s">
         <v>96</v>
       </c>
     </row>
@@ -9092,10 +9196,10 @@
       <c r="E257" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F257" s="76" t="s">
+      <c r="F257" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G257" s="76" t="s">
+      <c r="G257" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9115,10 +9219,10 @@
       <c r="E258" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F258" s="76" t="s">
+      <c r="F258" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G258" s="76" t="s">
+      <c r="G258" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9138,10 +9242,10 @@
       <c r="E259" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F259" s="76" t="s">
+      <c r="F259" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G259" s="76" t="s">
+      <c r="G259" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9161,10 +9265,10 @@
       <c r="E260" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F260" s="76" t="s">
+      <c r="F260" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G260" s="76" t="s">
+      <c r="G260" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9184,10 +9288,10 @@
       <c r="E261" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F261" s="76" t="s">
+      <c r="F261" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G261" s="76" t="s">
+      <c r="G261" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9207,10 +9311,10 @@
       <c r="E262" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F262" s="76" t="s">
+      <c r="F262" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G262" s="76" t="s">
+      <c r="G262" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9230,10 +9334,10 @@
       <c r="E263" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F263" s="76" t="s">
+      <c r="F263" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G263" s="76" t="s">
+      <c r="G263" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9253,10 +9357,10 @@
       <c r="E264" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F264" s="76" t="s">
+      <c r="F264" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G264" s="76" t="s">
+      <c r="G264" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9276,10 +9380,10 @@
       <c r="E265" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F265" s="76" t="s">
+      <c r="F265" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G265" s="76" t="s">
+      <c r="G265" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9299,10 +9403,10 @@
       <c r="E266" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F266" s="76" t="s">
+      <c r="F266" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G266" s="76" t="s">
+      <c r="G266" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9322,10 +9426,10 @@
       <c r="E267" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F267" s="76" t="s">
+      <c r="F267" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G267" s="76" t="s">
+      <c r="G267" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9345,10 +9449,10 @@
       <c r="E268" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F268" s="76" t="s">
+      <c r="F268" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G268" s="76" t="s">
+      <c r="G268" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9368,10 +9472,10 @@
       <c r="E269" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F269" s="76" t="s">
+      <c r="F269" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G269" s="76" t="s">
+      <c r="G269" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9391,10 +9495,10 @@
       <c r="E270" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F270" s="76" t="s">
+      <c r="F270" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G270" s="76" t="s">
+      <c r="G270" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9414,10 +9518,10 @@
       <c r="E271" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F271" s="76" t="s">
+      <c r="F271" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G271" s="76" t="s">
+      <c r="G271" s="75" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9437,217 +9541,217 @@
       <c r="E272" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F272" s="76" t="s">
+      <c r="F272" s="75" t="s">
         <v>98</v>
       </c>
-      <c r="G272" s="76" t="s">
+      <c r="G272" s="75" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="273" spans="1:7" ht="13">
-      <c r="A273" s="83">
-        <v>1</v>
-      </c>
-      <c r="B273" s="83">
-        <v>0</v>
-      </c>
-      <c r="C273" s="84">
-        <v>0</v>
-      </c>
-      <c r="D273" s="84">
-        <v>0</v>
-      </c>
-      <c r="E273" s="83" t="s">
+      <c r="A273" s="82">
+        <v>1</v>
+      </c>
+      <c r="B273" s="82">
+        <v>0</v>
+      </c>
+      <c r="C273" s="83">
+        <v>0</v>
+      </c>
+      <c r="D273" s="83">
+        <v>0</v>
+      </c>
+      <c r="E273" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F273" s="83" t="s">
+      <c r="F273" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G273" s="83" t="s">
+      <c r="G273" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="274" spans="1:7" ht="13">
-      <c r="A274" s="83">
-        <v>1</v>
-      </c>
-      <c r="B274" s="83">
+      <c r="A274" s="82">
+        <v>1</v>
+      </c>
+      <c r="B274" s="82">
         <v>30</v>
       </c>
-      <c r="C274" s="84">
+      <c r="C274" s="83">
         <v>1E-4</v>
       </c>
-      <c r="D274" s="84">
+      <c r="D274" s="83">
         <v>2.5000000000000001E-3</v>
       </c>
-      <c r="E274" s="83" t="s">
+      <c r="E274" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F274" s="83" t="s">
+      <c r="F274" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G274" s="83" t="s">
+      <c r="G274" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="275" spans="1:7" ht="13">
-      <c r="A275" s="83">
-        <v>1</v>
-      </c>
-      <c r="B275" s="83">
+      <c r="A275" s="82">
+        <v>1</v>
+      </c>
+      <c r="B275" s="82">
         <v>50</v>
       </c>
-      <c r="C275" s="84">
+      <c r="C275" s="83">
         <v>1E-3</v>
       </c>
-      <c r="D275" s="84">
+      <c r="D275" s="83">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E275" s="83" t="s">
+      <c r="E275" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F275" s="83" t="s">
+      <c r="F275" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G275" s="83" t="s">
+      <c r="G275" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="276" spans="1:7" ht="13">
-      <c r="A276" s="83">
-        <v>1</v>
-      </c>
-      <c r="B276" s="83">
+      <c r="A276" s="82">
+        <v>1</v>
+      </c>
+      <c r="B276" s="82">
         <v>100</v>
       </c>
-      <c r="C276" s="84">
+      <c r="C276" s="83">
         <v>0.01</v>
       </c>
-      <c r="D276" s="84">
+      <c r="D276" s="83">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="E276" s="83" t="s">
+      <c r="E276" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F276" s="83" t="s">
+      <c r="F276" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G276" s="83" t="s">
+      <c r="G276" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="277" spans="1:7" ht="13">
-      <c r="A277" s="83">
-        <v>1</v>
-      </c>
-      <c r="B277" s="83">
+      <c r="A277" s="82">
+        <v>1</v>
+      </c>
+      <c r="B277" s="82">
         <v>400</v>
       </c>
-      <c r="C277" s="84">
+      <c r="C277" s="83">
         <v>0.1</v>
       </c>
-      <c r="D277" s="84">
+      <c r="D277" s="83">
         <v>0.06</v>
       </c>
-      <c r="E277" s="83" t="s">
+      <c r="E277" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F277" s="83" t="s">
+      <c r="F277" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G277" s="83" t="s">
+      <c r="G277" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="278" spans="1:7" ht="13">
-      <c r="A278" s="83">
-        <v>1</v>
-      </c>
-      <c r="B278" s="83">
+      <c r="A278" s="82">
+        <v>1</v>
+      </c>
+      <c r="B278" s="82">
         <v>600</v>
       </c>
-      <c r="C278" s="84">
+      <c r="C278" s="83">
         <v>0.25</v>
       </c>
-      <c r="D278" s="84">
+      <c r="D278" s="83">
         <v>0.125</v>
       </c>
-      <c r="E278" s="83" t="s">
+      <c r="E278" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F278" s="83" t="s">
+      <c r="F278" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G278" s="83" t="s">
+      <c r="G278" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="279" spans="1:7" ht="13">
-      <c r="A279" s="83">
-        <v>1</v>
-      </c>
-      <c r="B279" s="83">
+      <c r="A279" s="82">
+        <v>1</v>
+      </c>
+      <c r="B279" s="82">
         <v>800</v>
       </c>
-      <c r="C279" s="84">
+      <c r="C279" s="83">
         <v>0.45</v>
       </c>
-      <c r="D279" s="84">
+      <c r="D279" s="83">
         <v>0.17499999999999999</v>
       </c>
-      <c r="E279" s="83" t="s">
+      <c r="E279" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F279" s="83" t="s">
+      <c r="F279" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G279" s="83" t="s">
+      <c r="G279" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="280" spans="1:7" ht="13">
-      <c r="A280" s="83">
-        <v>1</v>
-      </c>
-      <c r="B280" s="83">
+      <c r="A280" s="82">
+        <v>1</v>
+      </c>
+      <c r="B280" s="82">
         <v>1200</v>
       </c>
-      <c r="C280" s="84">
+      <c r="C280" s="83">
         <v>0.85</v>
       </c>
-      <c r="D280" s="84">
+      <c r="D280" s="83">
         <v>0.22500000000000001</v>
       </c>
-      <c r="E280" s="83" t="s">
+      <c r="E280" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F280" s="83" t="s">
+      <c r="F280" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G280" s="83" t="s">
+      <c r="G280" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="281" spans="1:7" ht="13">
-      <c r="A281" s="83">
-        <v>1</v>
-      </c>
-      <c r="B281" s="83">
+      <c r="A281" s="82">
+        <v>1</v>
+      </c>
+      <c r="B281" s="82">
         <v>1700</v>
       </c>
-      <c r="C281" s="84">
-        <v>1</v>
-      </c>
-      <c r="D281" s="84">
+      <c r="C281" s="83">
+        <v>1</v>
+      </c>
+      <c r="D281" s="83">
         <v>0.25</v>
       </c>
-      <c r="E281" s="83" t="s">
+      <c r="E281" s="82" t="s">
         <v>100</v>
       </c>
-      <c r="F281" s="83" t="s">
+      <c r="F281" s="82" t="s">
         <v>101</v>
       </c>
-      <c r="G281" s="83" t="s">
+      <c r="G281" s="82" t="s">
         <v>102</v>
       </c>
     </row>
@@ -9662,8 +9766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -9697,46 +9801,46 @@
       <c r="C1" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="71" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="I1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="K1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="L1" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="77" t="s">
+      <c r="M1" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="77" t="s">
+      <c r="N1" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="69" t="s">
+      <c r="O1" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="P1" s="69" t="s">
+      <c r="P1" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="Q1" s="70" t="s">
+      <c r="Q1" s="69" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9744,17 +9848,17 @@
       <c r="A2" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="73">
+      <c r="C2" s="72">
         <f>_measures_details!B15</f>
         <v>40572510.205771826</v>
       </c>
-      <c r="D2" s="78">
-        <v>1</v>
-      </c>
-      <c r="E2" s="74">
+      <c r="D2" s="77">
+        <v>1</v>
+      </c>
+      <c r="E2" s="73">
         <v>-1</v>
       </c>
       <c r="F2" s="59">
@@ -9778,10 +9882,10 @@
       <c r="L2" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="80" t="s">
+      <c r="M2" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="80">
+      <c r="N2" s="79">
         <v>0</v>
       </c>
       <c r="O2" s="59">
@@ -9805,7 +9909,7 @@
         <f>_measures_details!B26</f>
         <v>63968125.006875344</v>
       </c>
-      <c r="D3" s="78">
+      <c r="D3" s="77">
         <v>1</v>
       </c>
       <c r="E3" s="59">
@@ -9832,10 +9936,10 @@
       <c r="L3" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="80" t="s">
+      <c r="M3" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="80">
+      <c r="N3" s="79">
         <v>0</v>
       </c>
       <c r="O3" s="59">
@@ -9859,7 +9963,7 @@
         <f>_measures_details!B34</f>
         <v>22388843.752406374</v>
       </c>
-      <c r="D4" s="78">
+      <c r="D4" s="77">
         <v>1</v>
       </c>
       <c r="E4" s="59">
@@ -9886,10 +9990,10 @@
       <c r="L4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="M4" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="80">
+      <c r="N4" s="79">
         <v>0</v>
       </c>
       <c r="O4" s="59">
@@ -9913,7 +10017,7 @@
         <f>_measures_details!B43</f>
         <v>731904375.02062607</v>
       </c>
-      <c r="D5" s="78">
+      <c r="D5" s="77">
         <v>1</v>
       </c>
       <c r="E5" s="59">
@@ -9941,10 +10045,10 @@
       <c r="L5" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="80" t="s">
+      <c r="M5" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="80">
+      <c r="N5" s="79">
         <v>0</v>
       </c>
       <c r="O5" s="59">
@@ -9968,7 +10072,7 @@
         <f>_measures_details!B22</f>
         <v>3911963265.4766488</v>
       </c>
-      <c r="D6" s="78">
+      <c r="D6" s="77">
         <v>1</v>
       </c>
       <c r="E6" s="59">
@@ -9995,10 +10099,10 @@
       <c r="L6" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="80" t="s">
+      <c r="M6" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="80">
+      <c r="N6" s="79">
         <v>0</v>
       </c>
       <c r="O6" s="59">
@@ -10021,7 +10125,7 @@
       <c r="C7" s="63">
         <v>10000000</v>
       </c>
-      <c r="D7" s="78">
+      <c r="D7" s="77">
         <v>1</v>
       </c>
       <c r="E7" s="59">
@@ -10048,10 +10152,10 @@
       <c r="L7" s="59" t="s">
         <v>47</v>
       </c>
-      <c r="M7" s="80" t="s">
+      <c r="M7" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="80">
+      <c r="N7" s="79">
         <v>0</v>
       </c>
       <c r="O7" s="59">
@@ -10075,7 +10179,7 @@
         <f>1000000+2%*P8</f>
         <v>21000000</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="77">
         <v>1</v>
       </c>
       <c r="E8" s="59">
@@ -10102,10 +10206,10 @@
       <c r="L8" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="80" t="s">
+      <c r="M8" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="80">
+      <c r="N8" s="79">
         <v>0</v>
       </c>
       <c r="O8" s="61">
@@ -10141,10 +10245,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="70" t="s">
         <v>51</v>
       </c>
     </row>
@@ -12204,7 +12308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C13"/>
     </sheetView>
   </sheetViews>
@@ -14474,145 +14578,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="80" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="80" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="82">
-        <v>1</v>
-      </c>
-      <c r="C2" s="82" t="s">
+      <c r="A2" s="81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="81">
+        <v>1</v>
+      </c>
+      <c r="C2" s="81" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="82">
-        <v>1</v>
-      </c>
-      <c r="C3" s="82" t="s">
+      <c r="B3" s="81">
+        <v>1</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="82">
-        <v>0</v>
-      </c>
-      <c r="C4" s="82">
+      <c r="B4" s="81">
+        <v>0</v>
+      </c>
+      <c r="C4" s="81">
         <v>2017</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="82">
-        <v>1</v>
-      </c>
-      <c r="C5" s="82" t="s">
+      <c r="A5" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="81">
+        <v>1</v>
+      </c>
+      <c r="C5" s="81" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="82">
+      <c r="A6" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="81">
         <v>3</v>
       </c>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="81" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="82">
-        <v>1</v>
-      </c>
-      <c r="C7" s="82" t="s">
+      <c r="B7" s="81">
+        <v>1</v>
+      </c>
+      <c r="C7" s="81" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="81">
         <v>2</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="81" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="82" t="s">
+      <c r="A9" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="81">
         <v>3</v>
       </c>
-      <c r="C9" s="82" t="s">
+      <c r="C9" s="81" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="81">
         <v>4</v>
       </c>
-      <c r="C10" s="82" t="s">
+      <c r="C10" s="81" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="82">
+      <c r="B11" s="81">
         <v>5</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="81" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="81">
         <v>6</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="81" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="81">
         <v>7</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="81" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change if to impf in entity template
</commit_message>
<xml_diff>
--- a/data/system/entity_template.xlsx
+++ b/data/system/entity_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aznarsig/Documents/Python/climada_python/data/system/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zeliestalhanske/python_projects/climada_python/data/system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9E037C-4C3D-5640-AD3A-B2F8F9A96DD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E9B53B-009D-3C43-9278-0177C3B6A71F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="766" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1588,9 +1592,6 @@
     <t>risk transfer, demo</t>
   </si>
   <si>
-    <t>if_TC</t>
-  </si>
-  <si>
     <t>cover</t>
   </si>
   <si>
@@ -1615,9 +1616,6 @@
     <t>centr_TC</t>
   </si>
   <si>
-    <t>if_FL</t>
-  </si>
-  <si>
     <t>centr_FL</t>
   </si>
   <si>
@@ -1640,6 +1638,12 @@
   </si>
   <si>
     <t>risk transfer cost factor</t>
+  </si>
+  <si>
+    <t>impf_TC</t>
+  </si>
+  <si>
+    <t>impf_FL</t>
   </si>
 </sst>
 </file>
@@ -2358,8 +2362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="13"/>
@@ -2380,37 +2384,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="64" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="64" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" s="64" t="s">
-        <v>116</v>
-      </c>
-      <c r="D1" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="64" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="64" t="s">
+      <c r="H1" s="64" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="64" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="64" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="64" t="s">
+      <c r="J1" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="K1" s="64" t="s">
         <v>121</v>
-      </c>
-      <c r="J1" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="64" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -3304,22 +3308,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="49" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="E1" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" s="74" t="s">
         <v>125</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="E1" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="F1" s="74" t="s">
-        <v>127</v>
       </c>
       <c r="G1" s="74" t="s">
         <v>4</v>
@@ -9776,7 +9780,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -9852,7 +9856,7 @@
         <v>37</v>
       </c>
       <c r="Q1" s="87" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="R1" s="69" t="s">
         <v>3</v>

</xml_diff>